<commit_message>
Add Light off Command
</commit_message>
<xml_diff>
--- a/templates/export/group_device_report.xlsx
+++ b/templates/export/group_device_report.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syousuf/code/p/traccar/traccar/templates/export/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C771C8FB-E80B-8F44-91A7-FE0D0E26944E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="-21140" windowWidth="26220" windowHeight="16100" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="33600" windowHeight="19640" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -17,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Summary!$33:$40</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0">
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -67,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A41" authorId="0">
+    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -273,28 +269,6 @@
   </si>
   <si>
     <t>አቶ ሰናም አህመድ</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    ድርጅታችን ሰናም አህመድ አጠቃላይ አስመጪ ከመስረያቤታችሁ ጋር ባደረገው ወል መሰረት በ(</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Abyssinica SIL"/>
-      </rPr>
-      <t>${groupName}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Abyssinica SIL"/>
-      </rPr>
-      <t>) የሞተር ሳይክል ማህበር ከተደራጁ አባል መካከል ለ(${devicesCount}) ሞተር ሳይክል GPS የተገጠመላቸወ በመሆኑ እና በድርጅታችን website (monitor.ethiogps.com) ላይ የሚታዩ በመሆኑ መስሪያ ቤታችሁ የሚያስፈልገውን ሁሉ አንድያደርግላቸው በትህትና አንጠያቃለን።</t>
-    </r>
   </si>
   <si>
     <t>Group Name:</t>
@@ -331,11 +305,33 @@
       <t>${device.registrationSubCity}</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    ድርጅታችን ሰናም አህመድ አጠቃላይ አስመጪ ከመስረያቤታችሁ ጋር ባደረገው ወል መሰረት በ(</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Abyssinica SIL"/>
+      </rPr>
+      <t>${groupName}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Abyssinica SIL"/>
+      </rPr>
+      <t>) የሞተር ሳይክል ማህበር ከተደራጁ አባል መካከል ለ(${devicesCount}) ሞተር ሳይክል የተፈቀደላቸውን የፊጥነት ገደብ ሲያልፍ ቀይ መብራት የሚያበራ GPS የተገጠመላቸወ በመሆኑ እና በድርጅታችን website (monitor.ethiogps.com) ላይ የሚታዩ በመሆኑ መስሪያ ቤታችሁ የሚያስፈልገውን ሁሉ አንድያደርግላቸው በትህትና አንጠያቃለን።</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]&quot; h &quot;m&quot; min&quot;"/>
   </numFmts>
@@ -646,6 +642,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -675,9 +674,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -787,7 +783,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -830,7 +832,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1123,11 +1131,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O951"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleSheetLayoutView="124" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:G37"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="124" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1152,46 +1160,46 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:15" ht="54" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21"/>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="L3" s="28" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="L3" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
       <c r="O3" s="21"/>
     </row>
     <row r="4" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="12"/>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1199,26 +1207,26 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
@@ -1241,72 +1249,72 @@
       <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
+      <c r="B14" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
       <c r="O14" s="22"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
       <c r="O15" s="22"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
       <c r="O16" s="22"/>
     </row>
     <row r="17" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
       <c r="O17" s="22"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1406,42 +1414,42 @@
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="7"/>
@@ -1461,15 +1469,15 @@
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
@@ -1477,23 +1485,23 @@
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
       <c r="M36" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="N36" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="N36" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="O36" s="35"/>
+      <c r="O36" s="36"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13"/>
-      <c r="B37" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
+      <c r="B37" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
       <c r="J37" s="25"/>
@@ -2578,7 +2586,7 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N41" r:id="rId1"/>
+    <hyperlink ref="N41" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.42" right="0.35" top="0.06" bottom="1.03" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Show new plate number on reports
</commit_message>
<xml_diff>
--- a/templates/export/group_device_report.xlsx
+++ b/templates/export/group_device_report.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C771C8FB-E80B-8F44-91A7-FE0D0E26944E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2DCBC0-9574-8A47-AD8B-8EE167C12A6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="33600" windowHeight="19640" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,9 +117,6 @@
     <t>${device.gender}</t>
   </si>
   <si>
-    <t>${device.plateNumber}</t>
-  </si>
-  <si>
     <t>${device.vehicleModel}</t>
   </si>
   <si>
@@ -326,6 +323,9 @@
       </rPr>
       <t>) የሞተር ሳይክል ማህበር ከተደራጁ አባል መካከል ለ(${devicesCount}) ሞተር ሳይክል የተፈቀደላቸውን የፊጥነት ገደብ ሲያልፍ ቀይ መብራት የሚያበራ GPS የተገጠመላቸወ በመሆኑ እና በድርጅታችን website (monitor.ethiogps.com) ላይ የሚታዩ በመሆኑ መስሪያ ቤታችሁ የሚያስፈልገውን ሁሉ አንድያደርግላቸው በትህትና አንጠያቃለን።</t>
     </r>
+  </si>
+  <si>
+    <t>${device.finalPlateNumber}</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O951"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="124" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleSheetLayoutView="124" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1161,7 +1161,7 @@
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:15" ht="54" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -1181,13 +1181,13 @@
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21"/>
       <c r="C3" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
       <c r="L3" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
@@ -1196,7 +1196,7 @@
     <row r="4" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="12"/>
       <c r="L4" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M4" s="31"/>
       <c r="N4" s="31"/>
@@ -1208,7 +1208,7 @@
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N23" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1401,12 +1401,12 @@
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N27" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N28" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1415,7 +1415,7 @@
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="34"/>
       <c r="C33" s="34"/>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="34"/>
       <c r="C34" s="34"/>
@@ -1470,10 +1470,10 @@
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="35"/>
       <c r="E36" s="35"/>
@@ -1485,17 +1485,17 @@
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
       <c r="M36" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N36" s="36" t="s">
         <v>58</v>
-      </c>
-      <c r="N36" s="36" t="s">
-        <v>59</v>
       </c>
       <c r="O36" s="36"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13"/>
       <c r="B37" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="27"/>
@@ -1520,54 +1520,54 @@
     </row>
     <row r="39" spans="1:15" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="D39" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="I39" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G39" s="5" t="s">
+      <c r="J39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N39" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M39" s="5" t="s">
+      <c r="O39" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="N39" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="O39" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>0</v>
@@ -1576,16 +1576,16 @@
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>4</v>
@@ -1594,7 +1594,7 @@
         <v>5</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>8</v>
@@ -1606,7 +1606,7 @@
         <v>7</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O40" s="2" t="s">
         <v>2</v>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="41" spans="1:15" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>9</v>
@@ -1623,40 +1623,40 @@
         <v>10</v>
       </c>
       <c r="D41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="4" t="s">
+      <c r="G41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H41" s="3" t="s">
+      <c r="I41" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="J41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L41" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L41" s="3" t="s">
+      <c r="M41" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M41" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="N41" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>